<commit_message>
Updated ch6 results and graphics
</commit_message>
<xml_diff>
--- a/Chapter6/Res.xlsx
+++ b/Chapter6/Res.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilurquhart/Dropbox/git/book/Chapter6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\book\Chapter6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063F7768-B4AF-404E-B5F5-5EAE961C95A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27000" windowHeight="18180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="27000" windowHeight="18180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fkrst" sheetId="1" r:id="rId1"/>
     <sheet name="second" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>DijkstraBi</t>
   </si>
@@ -93,53 +92,74 @@
     <t>AStar</t>
   </si>
   <si>
-    <t>Nodes = 75050</t>
-  </si>
-  <si>
     <t>Nodes = 73642</t>
   </si>
   <si>
-    <t>Stats:</t>
-  </si>
-  <si>
     <t>Ways = 13467</t>
   </si>
   <si>
-    <t>Load time =55734</t>
-  </si>
-  <si>
     <t>Nodes,73642</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>3984466166:2407072781AStarBiDirectionaldistance</t>
   </si>
   <si>
     <t>Time</t>
   </si>
   <si>
-    <t>DijkstraBiDirectionaldistance</t>
-  </si>
-  <si>
-    <t>AStardistance</t>
-  </si>
-  <si>
-    <t>Dijkstradistance</t>
-  </si>
-  <si>
-    <t>DijkstraFlooddistance</t>
-  </si>
-  <si>
     <t>38826274:52047461AStarBiDirectionaldistance</t>
+  </si>
+  <si>
+    <t>Load time =77244</t>
+  </si>
+  <si>
+    <t>3984466166:52047461AStarBiDirectionaldistance</t>
+  </si>
+  <si>
+    <t>4611819743:3715514804AStarBiDirectionaldistance</t>
+  </si>
+  <si>
+    <t>4756281951:2508067364AStarBiDirectionaldistance</t>
+  </si>
+  <si>
+    <t>320845744:5363531156AStarBiDirectionaldistance</t>
+  </si>
+  <si>
+    <t>2407072781:29769767AStarBiDirectionaldistance</t>
+  </si>
+  <si>
+    <t>3073722023:4611819743AStarBiDirectionaldistance</t>
+  </si>
+  <si>
+    <t>1631995154:2420233344AStarBiDirectionaldistance</t>
+  </si>
+  <si>
+    <t>1815330260:3984466166AStarBiDirectionaldistance</t>
+  </si>
+  <si>
+    <t>Route</t>
+  </si>
+  <si>
+    <t>Dist</t>
+  </si>
+  <si>
+    <t>A*Bi</t>
+  </si>
+  <si>
+    <t>A*</t>
+  </si>
+  <si>
+    <t>Improve D</t>
+  </si>
+  <si>
+    <t>Improve T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,21 +476,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -478,7 +498,7 @@
         <v>54240</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -495,7 +515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="C5" t="s">
         <v>15</v>
       </c>
@@ -527,7 +547,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>1</v>
       </c>
@@ -565,7 +585,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>2</v>
       </c>
@@ -603,7 +623,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>3</v>
       </c>
@@ -641,7 +661,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>4</v>
       </c>
@@ -679,7 +699,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>5</v>
       </c>
@@ -717,7 +737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>6</v>
       </c>
@@ -755,7 +775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>7</v>
       </c>
@@ -793,7 +813,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>8</v>
       </c>
@@ -831,7 +851,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>9</v>
       </c>
@@ -869,7 +889,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>10</v>
       </c>
@@ -907,7 +927,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:12">
       <c r="C17">
         <f>AVERAGE(C6:C15)</f>
         <v>2.0243502467245991</v>
@@ -955,178 +975,561 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811DCCA2-7073-E448-A5C0-0C2D4D976B9B}">
-  <dimension ref="A1:U10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H9" sqref="H9:H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C2" s="1" t="s">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C3" s="1" t="s">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C5" s="1" t="s">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C7" s="1" t="s">
+      <c r="C8">
+        <v>8.7480575637764595</v>
+      </c>
+      <c r="D8">
+        <v>19937</v>
+      </c>
+      <c r="E8">
+        <v>8.7480575637764595</v>
+      </c>
+      <c r="F8">
+        <f>E8-C8</f>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>20989</v>
+      </c>
+      <c r="H8">
+        <f>G8/D8</f>
+        <v>1.0527662135727542</v>
+      </c>
+      <c r="I8">
+        <v>8.7480575637764595</v>
+      </c>
+      <c r="J8">
+        <v>2685</v>
+      </c>
+      <c r="K8" s="1">
+        <v>9.3272195049398992</v>
+      </c>
+      <c r="L8">
+        <v>2332</v>
+      </c>
+      <c r="M8">
+        <v>8.7948567202307508</v>
+      </c>
+      <c r="N8">
+        <v>30994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9">
+        <v>3.12410085901712</v>
+      </c>
+      <c r="D9">
+        <v>16873</v>
+      </c>
+      <c r="E9">
+        <v>3.12410085901712</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F17" si="0">E9-C9</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>9896</v>
+      </c>
+      <c r="H9">
+        <f>G9/D9</f>
+        <v>0.58649914063889053</v>
+      </c>
+      <c r="I9">
+        <v>3.12410085901712</v>
+      </c>
+      <c r="J9">
+        <v>22</v>
+      </c>
+      <c r="K9" s="1">
+        <v>5.2743222031651298</v>
+      </c>
+      <c r="L9">
+        <v>2634</v>
+      </c>
+      <c r="M9">
+        <v>3.37239442912017</v>
+      </c>
+      <c r="N9">
+        <v>12071</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C9">
-        <v>9.3272195049398992</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C10">
+        <v>4.4219312262122097</v>
+      </c>
+      <c r="D10">
+        <v>16859</v>
+      </c>
+      <c r="E10">
+        <v>4.4219312262122097</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>10978</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H16" si="1">G10/D10</f>
+        <v>0.65116554955809958</v>
+      </c>
+      <c r="I10">
+        <v>4.4219312262122097</v>
+      </c>
+      <c r="J10">
+        <v>403</v>
+      </c>
+      <c r="K10" s="1">
+        <v>9.4206778620853697</v>
+      </c>
+      <c r="L10">
+        <v>9970</v>
+      </c>
+      <c r="M10">
+        <v>4.4219312262122097</v>
+      </c>
+      <c r="N10">
+        <v>10589</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="E9">
-        <v>5847</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="C11">
+        <v>1.33783489804814</v>
+      </c>
+      <c r="D11">
+        <v>17274</v>
+      </c>
+      <c r="E11">
+        <v>1.33783489804814</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>2603</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0.15068889660761839</v>
+      </c>
+      <c r="I11">
+        <v>1.33783489804814</v>
+      </c>
+      <c r="J11">
+        <v>17</v>
+      </c>
+      <c r="K11">
+        <v>2.14842429526876</v>
+      </c>
+      <c r="L11">
+        <v>210</v>
+      </c>
+      <c r="M11">
+        <v>1.48441888344481</v>
+      </c>
+      <c r="N11">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="G9">
-        <v>8.7948567202307508</v>
-      </c>
-      <c r="H9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9">
-        <v>27014</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="C12">
+        <v>2.0977849984185699</v>
+      </c>
+      <c r="D12">
+        <v>21257</v>
+      </c>
+      <c r="E12">
+        <v>2.0977849984185699</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>7668</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>0.36072823070047516</v>
+      </c>
+      <c r="I12">
+        <v>2.0977849984185699</v>
+      </c>
+      <c r="J12">
+        <v>53</v>
+      </c>
+      <c r="K12">
+        <v>2.2011457659319502</v>
+      </c>
+      <c r="L12">
+        <v>39</v>
+      </c>
+      <c r="M12">
+        <v>2.0977849984185699</v>
+      </c>
+      <c r="N12">
+        <v>2662</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="K9">
-        <v>8.7480575637764595</v>
-      </c>
-      <c r="L9" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9">
-        <v>5029</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="C13">
+        <v>0.61331226007171102</v>
+      </c>
+      <c r="D13">
+        <v>18020</v>
+      </c>
+      <c r="E13">
+        <v>0.61331226007171102</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>458</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>2.541620421753607E-2</v>
+      </c>
+      <c r="I13">
+        <v>0.61331226007171102</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0.71766010930624702</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>0.61331226007171102</v>
+      </c>
+      <c r="N13">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="O9">
-        <v>8.7480575637764595</v>
-      </c>
-      <c r="P9" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q9">
-        <v>28289</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="C14">
+        <v>4.3736010721657204</v>
+      </c>
+      <c r="D14">
+        <v>20110</v>
+      </c>
+      <c r="E14">
+        <v>4.3736010721657204</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>11310</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>0.5624067628045748</v>
+      </c>
+      <c r="I14">
+        <v>4.3736010721657204</v>
+      </c>
+      <c r="J14">
+        <v>331</v>
+      </c>
+      <c r="K14">
+        <v>5.4441280138924597</v>
+      </c>
+      <c r="L14">
+        <v>1793</v>
+      </c>
+      <c r="M14">
+        <v>5.6170225866985</v>
+      </c>
+      <c r="N14">
+        <v>18027</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="S9">
-        <v>8.7480575637764595</v>
-      </c>
-      <c r="T9" t="s">
-        <v>27</v>
-      </c>
-      <c r="U9">
-        <v>38396</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C15">
+        <v>4.0995871014295897</v>
+      </c>
+      <c r="D15">
+        <v>19683</v>
+      </c>
+      <c r="E15">
+        <v>4.0995871014295897</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>14041</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0.71335670375450899</v>
+      </c>
+      <c r="I15">
+        <v>4.0995871014295897</v>
+      </c>
+      <c r="J15">
+        <v>215</v>
+      </c>
+      <c r="K15">
+        <v>4.2393357342909299</v>
+      </c>
+      <c r="L15">
+        <v>174</v>
+      </c>
+      <c r="M15">
+        <v>4.7198008889069802</v>
+      </c>
+      <c r="N15">
+        <v>12853</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C10">
-        <v>5.2743222031651298</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10">
-        <v>6723</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10">
-        <v>3.37239442912017</v>
-      </c>
-      <c r="H10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10">
-        <v>17261</v>
-      </c>
-      <c r="J10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10">
-        <v>3.12410085901712</v>
-      </c>
-      <c r="L10" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10">
-        <v>53</v>
-      </c>
-      <c r="N10" t="s">
-        <v>30</v>
-      </c>
-      <c r="O10">
-        <v>3.12410085901712</v>
-      </c>
-      <c r="P10" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q10">
-        <v>16017</v>
-      </c>
-      <c r="R10" t="s">
-        <v>31</v>
-      </c>
-      <c r="S10">
-        <v>3.12410085901712</v>
-      </c>
-      <c r="T10" t="s">
-        <v>27</v>
-      </c>
-      <c r="U10">
-        <v>37010</v>
+      <c r="C16">
+        <v>2.9251692704702998</v>
+      </c>
+      <c r="D16">
+        <v>18833</v>
+      </c>
+      <c r="E16">
+        <v>2.9251692704702998</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>14015</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0.74417246322943764</v>
+      </c>
+      <c r="I16">
+        <v>2.9251692704702998</v>
+      </c>
+      <c r="J16">
+        <v>203</v>
+      </c>
+      <c r="K16">
+        <v>3.1530949656176501</v>
+      </c>
+      <c r="L16">
+        <v>108</v>
+      </c>
+      <c r="M16">
+        <v>2.9978587683651101</v>
+      </c>
+      <c r="N16">
+        <v>7185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>4.2557433340954898</v>
+      </c>
+      <c r="D17">
+        <v>19043</v>
+      </c>
+      <c r="E17">
+        <v>4.2557433340954898</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>19006</v>
+      </c>
+      <c r="H17">
+        <f>G17/D17</f>
+        <v>0.9980570288294911</v>
+      </c>
+      <c r="I17">
+        <v>4.2557433340954898</v>
+      </c>
+      <c r="J17">
+        <v>71</v>
+      </c>
+      <c r="K17">
+        <v>5.4525008276846201</v>
+      </c>
+      <c r="L17">
+        <v>1418</v>
+      </c>
+      <c r="M17">
+        <v>4.1728692888343302</v>
+      </c>
+      <c r="N17">
+        <v>11272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ch6 - West Scot added
</commit_message>
<xml_diff>
--- a/Chapter6/Res.xlsx
+++ b/Chapter6/Res.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\book\Chapter6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilurquhart/Dropbox/git/book/Chapter6/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141C7123-AAC7-824F-99EE-B5C94443449E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="27000" windowHeight="18180" activeTab="1"/>
+    <workbookView xWindow="3020" yWindow="6480" windowWidth="27000" windowHeight="18180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fkrst" sheetId="1" r:id="rId1"/>
     <sheet name="second" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>DijkstraBi</t>
   </si>
@@ -92,9 +93,6 @@
     <t>AStar</t>
   </si>
   <si>
-    <t>Nodes = 73642</t>
-  </si>
-  <si>
     <t>Ways = 13467</t>
   </si>
   <si>
@@ -140,26 +138,29 @@
     <t>Route</t>
   </si>
   <si>
-    <t>Dist</t>
-  </si>
-  <si>
-    <t>A*Bi</t>
+    <t>Distance</t>
+  </si>
+  <si>
+    <t>Dijkstra B-Directional</t>
+  </si>
+  <si>
+    <t>A* Bi-Directional</t>
   </si>
   <si>
     <t>A*</t>
   </si>
   <si>
-    <t>Improve D</t>
-  </si>
-  <si>
-    <t>Improve T</t>
+    <t>Dijkstra Flood</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,9 +195,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,21 +479,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -498,7 +501,7 @@
         <v>54240</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -515,7 +518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>15</v>
       </c>
@@ -547,7 +550,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -585,7 +588,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -623,7 +626,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -661,7 +664,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -699,7 +702,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>5</v>
       </c>
@@ -737,7 +740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6</v>
       </c>
@@ -775,7 +778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>7</v>
       </c>
@@ -813,7 +816,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>8</v>
       </c>
@@ -851,7 +854,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>9</v>
       </c>
@@ -889,7 +892,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>10</v>
       </c>
@@ -927,7 +930,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="3:12">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C17">
         <f>AVERAGE(C6:C15)</f>
         <v>2.0243502467245991</v>
@@ -975,561 +978,780 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{811DCCA2-7073-E448-A5C0-0C2D4D976B9B}">
+  <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:H17"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="3">
+        <v>8.7480575637764595</v>
+      </c>
+      <c r="D6">
+        <v>19937</v>
+      </c>
+      <c r="F6" s="3">
+        <v>8.7480575637764595</v>
+      </c>
+      <c r="G6">
+        <v>20989</v>
+      </c>
+      <c r="H6">
+        <f>1-(G6/D6)</f>
+        <v>-5.2766213572754239E-2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>8.7480575637764595</v>
+      </c>
+      <c r="J6">
+        <v>2685</v>
+      </c>
+      <c r="K6">
+        <f>1-(J6/D6)</f>
+        <v>0.86532577619501427</v>
+      </c>
+      <c r="L6" s="2">
+        <v>9.3272195049398992</v>
+      </c>
+      <c r="M6" s="2">
+        <f>1-(L6/C6)</f>
+        <v>-6.6204633078959851E-2</v>
+      </c>
+      <c r="N6">
+        <v>2332</v>
+      </c>
+      <c r="O6">
+        <f>1-(N6/D6)</f>
+        <v>0.88303154938054873</v>
+      </c>
+      <c r="P6" s="3">
+        <v>8.7948567202307508</v>
+      </c>
+      <c r="Q6" s="3">
+        <f>1-(P6/C6)</f>
+        <v>-5.3496626094546862E-3</v>
+      </c>
+      <c r="R6">
+        <v>30994</v>
+      </c>
+      <c r="S6">
+        <f>1-(R6/D6)</f>
+        <v>-0.55459698048853889</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.12410085901712</v>
+      </c>
+      <c r="D7">
+        <v>16873</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3.12410085901712</v>
+      </c>
+      <c r="G7">
+        <v>9896</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H15" si="0">1-(G7/D7)</f>
+        <v>0.41350085936110947</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3.12410085901712</v>
+      </c>
+      <c r="J7">
+        <v>22</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:K15" si="1">1-(J7/D7)</f>
+        <v>0.99869614176494992</v>
+      </c>
+      <c r="L7" s="2">
+        <v>5.2743222031651298</v>
+      </c>
+      <c r="M7" s="2">
+        <f t="shared" ref="M7:M15" si="2">1-(L7/C7)</f>
+        <v>-0.68826886236460871</v>
+      </c>
+      <c r="N7">
+        <v>2634</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:O15" si="3">1-(N7/D7)</f>
+        <v>0.84389260949445855</v>
+      </c>
+      <c r="P7" s="3">
+        <v>3.37239442912017</v>
+      </c>
+      <c r="Q7" s="3">
+        <f t="shared" ref="Q7:Q15" si="4">1-(P7/C7)</f>
+        <v>-7.947680990720829E-2</v>
+      </c>
+      <c r="R7">
+        <v>12071</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ref="S7:S15" si="5">1-(R7/D7)</f>
+        <v>0.28459669294138568</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C8" s="3">
+        <v>4.4219312262122097</v>
+      </c>
+      <c r="D8">
+        <v>16859</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4.4219312262122097</v>
+      </c>
+      <c r="G8">
+        <v>10978</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.34883445044190042</v>
+      </c>
+      <c r="I8" s="3">
+        <v>4.4219312262122097</v>
+      </c>
+      <c r="J8">
+        <v>403</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0.97609585384661013</v>
+      </c>
+      <c r="L8" s="2">
+        <v>9.4206778620853697</v>
+      </c>
+      <c r="M8" s="2">
+        <f t="shared" si="2"/>
+        <v>-1.1304442290376926</v>
+      </c>
+      <c r="N8">
+        <v>9970</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="3"/>
+        <v>0.40862447357494514</v>
+      </c>
+      <c r="P8" s="3">
+        <v>4.4219312262122097</v>
+      </c>
+      <c r="Q8" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>10589</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="5"/>
+        <v>0.37190817960733136</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.33783489804814</v>
+      </c>
+      <c r="D9">
+        <v>17274</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.33783489804814</v>
+      </c>
+      <c r="G9">
+        <v>2603</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.84931110339238158</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.33783489804814</v>
+      </c>
+      <c r="J9">
+        <v>17</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>0.99901586198911663</v>
+      </c>
+      <c r="L9" s="2">
+        <v>2.14842429526876</v>
+      </c>
+      <c r="M9" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.60589643640126667</v>
+      </c>
+      <c r="N9">
+        <v>210</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="3"/>
+        <v>0.98784300104202849</v>
+      </c>
+      <c r="P9" s="3">
+        <v>1.48441888344481</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.10956806823512477</v>
+      </c>
+      <c r="R9">
+        <v>1361</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="5"/>
+        <v>0.92121106865809887</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2.0977849984185699</v>
+      </c>
+      <c r="D10">
+        <v>21257</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2.0977849984185699</v>
+      </c>
+      <c r="G10">
+        <v>7668</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.63927176929952489</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2.0977849984185699</v>
+      </c>
+      <c r="J10">
+        <v>53</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>0.99750670367408378</v>
+      </c>
+      <c r="L10" s="3">
+        <v>2.2011457659319502</v>
+      </c>
+      <c r="M10" s="2">
+        <f t="shared" si="2"/>
+        <v>-4.9271382716198131E-2</v>
+      </c>
+      <c r="N10">
+        <v>39</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="3"/>
+        <v>0.99816531025074096</v>
+      </c>
+      <c r="P10" s="3">
+        <v>2.0977849984185699</v>
+      </c>
+      <c r="Q10" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>2662</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="5"/>
+        <v>0.87477066378134261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.61331226007171102</v>
+      </c>
+      <c r="D11">
+        <v>18020</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.61331226007171102</v>
+      </c>
+      <c r="G11">
+        <v>458</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.9745837957824639</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.61331226007171102</v>
+      </c>
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="I6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0.9999445061043285</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.71766010930624702</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.17013820858943074</v>
+      </c>
+      <c r="N11">
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="3"/>
+        <v>0.99983351831298561</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.61331226007171102</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" t="s">
-        <v>35</v>
-      </c>
-      <c r="N7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8">
-        <v>8.7480575637764595</v>
-      </c>
-      <c r="D8">
-        <v>19937</v>
-      </c>
-      <c r="E8">
-        <v>8.7480575637764595</v>
-      </c>
-      <c r="F8">
-        <f>E8-C8</f>
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>20989</v>
-      </c>
-      <c r="H8">
-        <f>G8/D8</f>
-        <v>1.0527662135727542</v>
-      </c>
-      <c r="I8">
-        <v>8.7480575637764595</v>
-      </c>
-      <c r="J8">
-        <v>2685</v>
-      </c>
-      <c r="K8" s="1">
-        <v>9.3272195049398992</v>
-      </c>
-      <c r="L8">
-        <v>2332</v>
-      </c>
-      <c r="M8">
-        <v>8.7948567202307508</v>
-      </c>
-      <c r="N8">
-        <v>30994</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9">
-        <v>3.12410085901712</v>
-      </c>
-      <c r="D9">
-        <v>16873</v>
-      </c>
-      <c r="E9">
-        <v>3.12410085901712</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F17" si="0">E9-C9</f>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>9896</v>
-      </c>
-      <c r="H9">
-        <f>G9/D9</f>
-        <v>0.58649914063889053</v>
-      </c>
-      <c r="I9">
-        <v>3.12410085901712</v>
-      </c>
-      <c r="J9">
-        <v>22</v>
-      </c>
-      <c r="K9" s="1">
-        <v>5.2743222031651298</v>
-      </c>
-      <c r="L9">
-        <v>2634</v>
-      </c>
-      <c r="M9">
-        <v>3.37239442912017</v>
-      </c>
-      <c r="N9">
-        <v>12071</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10">
-        <v>4.4219312262122097</v>
-      </c>
-      <c r="D10">
-        <v>16859</v>
-      </c>
-      <c r="E10">
-        <v>4.4219312262122097</v>
-      </c>
-      <c r="F10">
+      <c r="R11">
+        <v>275</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="5"/>
+        <v>0.98473917869034411</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4.3736010721657204</v>
+      </c>
+      <c r="D12">
+        <v>20110</v>
+      </c>
+      <c r="F12" s="3">
+        <v>4.3736010721657204</v>
+      </c>
+      <c r="G12">
+        <v>11310</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>10978</v>
-      </c>
-      <c r="H10">
-        <f t="shared" ref="H10:H16" si="1">G10/D10</f>
-        <v>0.65116554955809958</v>
-      </c>
-      <c r="I10">
-        <v>4.4219312262122097</v>
-      </c>
-      <c r="J10">
-        <v>403</v>
-      </c>
-      <c r="K10" s="1">
-        <v>9.4206778620853697</v>
-      </c>
-      <c r="L10">
-        <v>9970</v>
-      </c>
-      <c r="M10">
-        <v>4.4219312262122097</v>
-      </c>
-      <c r="N10">
-        <v>10589</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11">
-        <v>1.33783489804814</v>
-      </c>
-      <c r="D11">
-        <v>17274</v>
-      </c>
-      <c r="E11">
-        <v>1.33783489804814</v>
-      </c>
-      <c r="F11">
+        <v>0.4375932371954252</v>
+      </c>
+      <c r="I12" s="3">
+        <v>4.3736010721657204</v>
+      </c>
+      <c r="J12">
+        <v>331</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>0.98354052710094475</v>
+      </c>
+      <c r="L12" s="3">
+        <v>5.4441280138924597</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.24477013885416743</v>
+      </c>
+      <c r="N12">
+        <v>1793</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="3"/>
+        <v>0.91084037792143213</v>
+      </c>
+      <c r="P12" s="3">
+        <v>5.6170225866985</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.28430153871282604</v>
+      </c>
+      <c r="R12">
+        <v>18027</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="5"/>
+        <v>0.10358030830432619</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4.0995871014295897</v>
+      </c>
+      <c r="D13">
+        <v>19683</v>
+      </c>
+      <c r="F13" s="3">
+        <v>4.0995871014295897</v>
+      </c>
+      <c r="G13">
+        <v>14041</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>2603</v>
-      </c>
-      <c r="H11">
+        <v>0.28664329624549101</v>
+      </c>
+      <c r="I13" s="3">
+        <v>4.0995871014295897</v>
+      </c>
+      <c r="J13">
+        <v>215</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="1"/>
-        <v>0.15068889660761839</v>
-      </c>
-      <c r="I11">
-        <v>1.33783489804814</v>
-      </c>
-      <c r="J11">
-        <v>17</v>
-      </c>
-      <c r="K11">
-        <v>2.14842429526876</v>
-      </c>
-      <c r="L11">
-        <v>210</v>
-      </c>
-      <c r="M11">
-        <v>1.48441888344481</v>
-      </c>
-      <c r="N11">
-        <v>1361</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <v>2.0977849984185699</v>
-      </c>
-      <c r="D12">
-        <v>21257</v>
-      </c>
-      <c r="E12">
-        <v>2.0977849984185699</v>
-      </c>
-      <c r="F12">
+        <v>0.98907686836356246</v>
+      </c>
+      <c r="L13" s="3">
+        <v>4.2393357342909299</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="2"/>
+        <v>-3.4088465351207686E-2</v>
+      </c>
+      <c r="N13">
+        <v>174</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="3"/>
+        <v>0.99115988416399936</v>
+      </c>
+      <c r="P13" s="3">
+        <v>4.7198008889069802</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" si="4"/>
+        <v>-0.15128689112645333</v>
+      </c>
+      <c r="R13">
+        <v>12853</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="5"/>
+        <v>0.34699994919473653</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2.9251692704702998</v>
+      </c>
+      <c r="D14">
+        <v>18833</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2.9251692704702998</v>
+      </c>
+      <c r="G14">
+        <v>14015</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>7668</v>
-      </c>
-      <c r="H12">
+        <v>0.25582753677056236</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2.9251692704702998</v>
+      </c>
+      <c r="J14">
+        <v>203</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="1"/>
-        <v>0.36072823070047516</v>
-      </c>
-      <c r="I12">
-        <v>2.0977849984185699</v>
-      </c>
-      <c r="J12">
-        <v>53</v>
-      </c>
-      <c r="K12">
-        <v>2.2011457659319502</v>
-      </c>
-      <c r="L12">
-        <v>39</v>
-      </c>
-      <c r="M12">
-        <v>2.0977849984185699</v>
-      </c>
-      <c r="N12">
-        <v>2662</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13">
-        <v>0.61331226007171102</v>
-      </c>
-      <c r="D13">
-        <v>18020</v>
-      </c>
-      <c r="E13">
-        <v>0.61331226007171102</v>
-      </c>
-      <c r="F13">
+        <v>0.98922104816014444</v>
+      </c>
+      <c r="L14" s="3">
+        <v>3.1530949656176501</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="2"/>
+        <v>-7.7918805399834312E-2</v>
+      </c>
+      <c r="N14">
+        <v>108</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="3"/>
+        <v>0.99426538522805719</v>
+      </c>
+      <c r="P14" s="3">
+        <v>2.9978587683651101</v>
+      </c>
+      <c r="Q14" s="3">
+        <f t="shared" si="4"/>
+        <v>-2.4849672334730677E-2</v>
+      </c>
+      <c r="R14">
+        <v>7185</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="5"/>
+        <v>0.61848882281102324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="3">
+        <v>4.2557433340954898</v>
+      </c>
+      <c r="D15">
+        <v>19043</v>
+      </c>
+      <c r="F15" s="3">
+        <v>4.2557433340954898</v>
+      </c>
+      <c r="G15">
+        <v>19006</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>458</v>
-      </c>
-      <c r="H13">
+        <v>1.9429711705089003E-3</v>
+      </c>
+      <c r="I15" s="3">
+        <v>4.2557433340954898</v>
+      </c>
+      <c r="J15">
+        <v>71</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="1"/>
-        <v>2.541620421753607E-2</v>
-      </c>
-      <c r="I13">
-        <v>0.61331226007171102</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>0.71766010930624702</v>
-      </c>
-      <c r="L13">
-        <v>3</v>
-      </c>
-      <c r="M13">
-        <v>0.61331226007171102</v>
-      </c>
-      <c r="N13">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14">
-        <v>4.3736010721657204</v>
-      </c>
-      <c r="D14">
-        <v>20110</v>
-      </c>
-      <c r="E14">
-        <v>4.3736010721657204</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>11310</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="1"/>
-        <v>0.5624067628045748</v>
-      </c>
-      <c r="I14">
-        <v>4.3736010721657204</v>
-      </c>
-      <c r="J14">
-        <v>331</v>
-      </c>
-      <c r="K14">
-        <v>5.4441280138924597</v>
-      </c>
-      <c r="L14">
-        <v>1793</v>
-      </c>
-      <c r="M14">
-        <v>5.6170225866985</v>
-      </c>
-      <c r="N14">
-        <v>18027</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15">
-        <v>4.0995871014295897</v>
-      </c>
-      <c r="D15">
-        <v>19683</v>
-      </c>
-      <c r="E15">
-        <v>4.0995871014295897</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>14041</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="1"/>
-        <v>0.71335670375450899</v>
-      </c>
-      <c r="I15">
-        <v>4.0995871014295897</v>
-      </c>
-      <c r="J15">
-        <v>215</v>
-      </c>
-      <c r="K15">
-        <v>4.2393357342909299</v>
-      </c>
-      <c r="L15">
-        <v>174</v>
-      </c>
-      <c r="M15">
-        <v>4.7198008889069802</v>
+        <v>0.99627159586199654</v>
+      </c>
+      <c r="L15" s="3">
+        <v>5.4525008276846201</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="2"/>
+        <v>-0.28120997899500622</v>
       </c>
       <c r="N15">
-        <v>12853</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16">
-        <v>2.9251692704702998</v>
-      </c>
-      <c r="D16">
-        <v>18833</v>
-      </c>
-      <c r="E16">
-        <v>2.9251692704702998</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>14015</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="1"/>
-        <v>0.74417246322943764</v>
-      </c>
-      <c r="I16">
-        <v>2.9251692704702998</v>
-      </c>
-      <c r="J16">
-        <v>203</v>
-      </c>
-      <c r="K16">
-        <v>3.1530949656176501</v>
-      </c>
-      <c r="L16">
-        <v>108</v>
-      </c>
-      <c r="M16">
-        <v>2.9978587683651101</v>
-      </c>
-      <c r="N16">
-        <v>7185</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17">
-        <v>4.2557433340954898</v>
-      </c>
-      <c r="D17">
-        <v>19043</v>
-      </c>
-      <c r="E17">
-        <v>4.2557433340954898</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>19006</v>
-      </c>
-      <c r="H17">
-        <f>G17/D17</f>
-        <v>0.9980570288294911</v>
-      </c>
-      <c r="I17">
-        <v>4.2557433340954898</v>
-      </c>
-      <c r="J17">
-        <v>71</v>
-      </c>
-      <c r="K17">
-        <v>5.4525008276846201</v>
-      </c>
-      <c r="L17">
         <v>1418</v>
       </c>
-      <c r="M17">
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>0.92553694270860687</v>
+      </c>
+      <c r="P15" s="3">
         <v>4.1728692888343302</v>
       </c>
-      <c r="N17">
+      <c r="Q15" s="3">
+        <f t="shared" si="4"/>
+        <v>1.9473459453534847E-2</v>
+      </c>
+      <c r="R15">
         <v>11272</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="5"/>
+        <v>0.40807645854119623</v>
+      </c>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C17" s="3">
+        <f>AVERAGE(C6:C15)</f>
+        <v>3.5997122583705305</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" ref="D17:R17" si="6">AVERAGE(D6:D15)</f>
+        <v>18788.900000000001</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3">
+        <f t="shared" si="6"/>
+        <v>3.5997122583705305</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="6"/>
+        <v>11096.4</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3">
+        <f t="shared" si="6"/>
+        <v>3.5997122583705305</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="6"/>
+        <v>400.1</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="6"/>
+        <v>0.97946948830607516</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" si="6"/>
+        <v>4.7378509282183021</v>
+      </c>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3">
+        <f t="shared" si="6"/>
+        <v>1868.1</v>
+      </c>
+      <c r="O17" s="3">
+        <f t="shared" si="6"/>
+        <v>0.89431930520778047</v>
+      </c>
+      <c r="P17" s="3">
+        <f t="shared" si="6"/>
+        <v>3.8292250050303145</v>
+      </c>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3">
+        <f t="shared" si="6"/>
+        <v>10728.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>